<commit_message>
Fix lỗi chính tả
</commit_message>
<xml_diff>
--- a/5_TaskList/Lịch làm việc.xlsx
+++ b/5_TaskList/Lịch làm việc.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhamAnhPhu_Fit\5_TaskList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPTS\Fit-thuctap\Fit-thuctap\5_TaskList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E482A5B7-6B9E-43F3-A2A1-A2CCF4B9B9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Lịch làm việc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -64,44 +63,49 @@
     </r>
   </si>
   <si>
-    <t>- Đọc tài liệu .Net và Oracle. làm các phần bài tập cuối chương các chương 1 - 6  cảu Oracle.</t>
-  </si>
-  <si>
-    <t>- Đọc tài liệu và làm các phần bài tập cuối chương 7-9 của Oracle. Nộp bài tập chương 1-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đọc tài liệu và làm các bài tập cuối chương 1-4 của ASP.Net. Nộp bài tập chương 9 của Oracle, chương 1-3 của ASP.Net.F11  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đọc tài liệu chương 5-6 của ASP.Net. Nộp bài tập chương 5 của ASP.Net. </t>
-  </si>
-  <si>
-    <t>Đọc tài liệu và làm bài tập chương 7 của ASP.Net. Tham gia tổ chức 20/10 tại công ty</t>
-  </si>
-  <si>
-    <t>Làm bài Exam 2,Exam3 của Oracle</t>
-  </si>
-  <si>
-    <t>Làm bài Exam 1,Exam 2 cảu Oracle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Làm Exam 1 của Asp.Net </t>
-  </si>
-  <si>
-    <t>Làm tiếp Exam 1 và làm lại bài tập của Asp.Net</t>
+    <t>- Đọc tài liệu .Net và Oracle. 
+- Làm các phần bài tập cuối chương: chương 1 - 6  của Oracle.</t>
+  </si>
+  <si>
+    <t>- Đọc tài liệu và làm các phần bài tập cuối chương 7-9 của Oracle. 
+- Nộp bài tập chương 1-8</t>
+  </si>
+  <si>
+    <t>- Đọc tài liệu và làm các bài tập cuối chương 1-4 của ASP.Net. 
+- Nộp bài tập chương 9 của Oracle, chương 1-3 của ASP.Net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Đọc tài liệu chương 5-6 của ASP.Net. 
+- Nộp bài tập chương 5 của ASP.Net. </t>
+  </si>
+  <si>
+    <t>- Đọc tài liệu và làm bài tập chương 7 của ASP.Net. 
+- Tham gia tổ chức 20/10 tại công ty</t>
+  </si>
+  <si>
+    <t>- Làm bài Exam 1, Exam 2 của Oracle</t>
+  </si>
+  <si>
+    <t>- Làm bài Exam 2, Exa m3 của Oracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Làm Exam 1 của Asp.Net </t>
+  </si>
+  <si>
+    <t>- Làm tiếp Exam 1 và làm lại bài tập của Asp.Net</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="dd&quot; &quot;mmm"/>
     <numFmt numFmtId="165" formatCode="m&quot;/&quot;d"/>
     <numFmt numFmtId="166" formatCode="dd&quot;/&quot;mm"/>
     <numFmt numFmtId="167" formatCode="h&quot;:&quot;mm&quot; &quot;AM/PM&quot; &quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -559,29 +563,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="5" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="14" customFormat="1" ht="22.95" customHeight="1">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -597,7 +601,7 @@
       <c r="I1" s="17"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="36" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2">
@@ -630,7 +634,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="22.5" customHeight="1">
       <c r="A3" s="3"/>
       <c r="C3" s="4" t="str">
         <f t="shared" ref="C3:I3" si="0">UPPER(TEXT(C2, "DDDD"))</f>
@@ -662,7 +666,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="107.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="107.4" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -682,7 +686,7 @@
       </c>
       <c r="J4" s="8"/>
     </row>
-    <row r="8" spans="1:10" s="14" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" s="14" customFormat="1" ht="22.95" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>1</v>
@@ -698,7 +702,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="36" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2">
@@ -731,7 +735,7 @@
       </c>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="22.5" customHeight="1">
       <c r="A10" s="3"/>
       <c r="C10" s="4" t="str">
         <f t="shared" ref="C10:I10" si="1">UPPER(TEXT(C9, "DDDD"))</f>
@@ -763,7 +767,7 @@
       </c>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="105.6">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
@@ -772,16 +776,16 @@
       <c r="D11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="7" t="s">
@@ -789,7 +793,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="15" spans="1:10" s="14" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" s="14" customFormat="1" ht="22.95" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>2</v>
@@ -805,7 +809,7 @@
       <c r="I15" s="17"/>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="36" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2">
@@ -838,7 +842,7 @@
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="22.5" customHeight="1">
       <c r="A17" s="3"/>
       <c r="C17" s="4" t="str">
         <f t="shared" ref="C17:I17" si="2">UPPER(TEXT(C16, "DDDD"))</f>
@@ -870,25 +874,25 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="66.75" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="15" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="7" t="s">
@@ -896,7 +900,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="22" spans="1:10" s="14" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" s="14" customFormat="1" ht="22.95" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="10" t="s">
         <v>3</v>
@@ -912,7 +916,7 @@
       <c r="I22" s="17"/>
       <c r="J22" s="13"/>
     </row>
-    <row r="23" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="36" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2">
@@ -945,7 +949,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="22.5" customHeight="1">
       <c r="A24" s="3"/>
       <c r="C24" s="4" t="str">
         <f t="shared" ref="C24:I24" si="3">UPPER(TEXT(C23, "DDDD"))</f>
@@ -977,7 +981,7 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="98.25" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7" t="s">
@@ -991,7 +995,7 @@
       <c r="I25" s="7"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="29" spans="1:10" s="14" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" s="14" customFormat="1" ht="22.95" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="10" t="s">
         <v>4</v>
@@ -1007,7 +1011,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="36" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2">
@@ -1040,7 +1044,7 @@
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="22.5" customHeight="1">
       <c r="A31" s="3"/>
       <c r="C31" s="4" t="str">
         <f t="shared" ref="C31:I31" si="4">UPPER(TEXT(C30, "DDDD"))</f>
@@ -1072,7 +1076,7 @@
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="22.5" customHeight="1">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -1084,7 +1088,7 @@
       <c r="I32" s="7"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="36" spans="1:10" s="14" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" s="14" customFormat="1" ht="22.95" customHeight="1">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>5</v>
@@ -1100,7 +1104,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="36" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2">
@@ -1133,7 +1137,7 @@
       </c>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="22.5" customHeight="1">
       <c r="A38" s="3"/>
       <c r="C38" s="4" t="str">
         <f t="shared" ref="C38:I38" si="5">UPPER(TEXT(C37, "DDDD"))</f>
@@ -1165,7 +1169,7 @@
       </c>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="22.5" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>

</xml_diff>

<commit_message>
Update LichLamViec 29/12 - 3/1
</commit_message>
<xml_diff>
--- a/5_TaskList/Lịch làm việc.xlsx
+++ b/5_TaskList/Lịch làm việc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
   <si>
     <t xml:space="preserve">Tuần: 01
 </t>
@@ -245,6 +245,18 @@
   <si>
     <t xml:space="preserve">Tuần: 12
 </t>
+  </si>
+  <si>
+    <t>Thêm trang điều chỉnh hạn mức theo danh sách (làm các chức năng import, cập nhật, làm mới)</t>
+  </si>
+  <si>
+    <t>Sửa lỗi kiểm tra định dạng dữ liệu trong file import, gửi thông báo lên Topics</t>
+  </si>
+  <si>
+    <t>Thêm check file rỗng, không có dữ liệu, không có Header, sửa lỗi đọc cả các dòng thay đôi format. Nghỉ chiều..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiểm tra và sửa lại, đẩy code lên. Thêm check thêm file lỗi mà vẫn nhân cập nhật, </t>
   </si>
 </sst>
 </file>
@@ -268,10 +280,12 @@
       <sz val="16"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -481,17 +495,17 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="L88" sqref="L88"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -740,10 +754,10 @@
         <v>45571</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="25"/>
       <c r="J1" s="5"/>
       <c r="K1" s="6"/>
@@ -860,10 +874,10 @@
         <v>45578</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="25"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
@@ -986,10 +1000,10 @@
         <v>45585</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="25"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
@@ -1112,10 +1126,10 @@
         <v>45592</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="25"/>
       <c r="J22" s="5"/>
       <c r="K22" s="6"/>
@@ -1238,10 +1252,10 @@
         <v>45599</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="25"/>
       <c r="J29" s="5"/>
       <c r="K29" s="6"/>
@@ -1364,10 +1378,10 @@
         <v>45606</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
       <c r="I36" s="25"/>
       <c r="J36" s="5"/>
       <c r="K36" s="6"/>
@@ -1491,10 +1505,10 @@
         <v>45613</v>
       </c>
       <c r="D44" s="4"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
       <c r="I44" s="25"/>
       <c r="J44" s="5"/>
       <c r="K44" s="6"/>
@@ -1585,7 +1599,7 @@
       </c>
       <c r="J46" s="9"/>
     </row>
-    <row r="47" spans="1:32" ht="89.25">
+    <row r="47" spans="1:32" ht="76.5">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
       <c r="C47" s="19" t="s">
@@ -1623,17 +1637,17 @@
         <v>45620</v>
       </c>
       <c r="D51" s="22"/>
-      <c r="E51" s="26"/>
+      <c r="E51" s="24"/>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="25"/>
       <c r="I51" s="25"/>
-      <c r="J51" s="26"/>
+      <c r="J51" s="24"/>
       <c r="K51" s="25"/>
       <c r="L51" s="25"/>
       <c r="M51" s="25"/>
       <c r="N51" s="25"/>
-      <c r="O51" s="26"/>
+      <c r="O51" s="24"/>
       <c r="P51" s="25"/>
       <c r="Q51" s="25"/>
       <c r="R51" s="25"/>
@@ -1740,17 +1754,17 @@
         <v>45627</v>
       </c>
       <c r="D59" s="22"/>
-      <c r="E59" s="26"/>
+      <c r="E59" s="24"/>
       <c r="F59" s="25"/>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
       <c r="I59" s="25"/>
-      <c r="J59" s="26"/>
+      <c r="J59" s="24"/>
       <c r="K59" s="25"/>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
       <c r="N59" s="25"/>
-      <c r="O59" s="26"/>
+      <c r="O59" s="24"/>
       <c r="P59" s="25"/>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -1857,17 +1871,17 @@
         <v>45634</v>
       </c>
       <c r="D67" s="22"/>
-      <c r="E67" s="26"/>
+      <c r="E67" s="24"/>
       <c r="F67" s="25"/>
       <c r="G67" s="25"/>
       <c r="H67" s="25"/>
       <c r="I67" s="25"/>
-      <c r="J67" s="26"/>
+      <c r="J67" s="24"/>
       <c r="K67" s="25"/>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
       <c r="N67" s="25"/>
-      <c r="O67" s="26"/>
+      <c r="O67" s="24"/>
       <c r="P67" s="25"/>
       <c r="Q67" s="25"/>
       <c r="R67" s="25"/>
@@ -1974,17 +1988,17 @@
         <v>45641</v>
       </c>
       <c r="D75" s="22"/>
-      <c r="E75" s="26"/>
+      <c r="E75" s="24"/>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
       <c r="H75" s="25"/>
       <c r="I75" s="25"/>
-      <c r="J75" s="26"/>
+      <c r="J75" s="24"/>
       <c r="K75" s="25"/>
       <c r="L75" s="25"/>
       <c r="M75" s="25"/>
       <c r="N75" s="25"/>
-      <c r="O75" s="26"/>
+      <c r="O75" s="24"/>
       <c r="P75" s="25"/>
       <c r="Q75" s="25"/>
       <c r="R75" s="25"/>
@@ -2091,17 +2105,17 @@
         <v>45648</v>
       </c>
       <c r="D83" s="22"/>
-      <c r="E83" s="26"/>
+      <c r="E83" s="24"/>
       <c r="F83" s="25"/>
       <c r="G83" s="25"/>
       <c r="H83" s="25"/>
       <c r="I83" s="25"/>
-      <c r="J83" s="26"/>
+      <c r="J83" s="24"/>
       <c r="K83" s="25"/>
       <c r="L83" s="25"/>
       <c r="M83" s="25"/>
       <c r="N83" s="25"/>
-      <c r="O83" s="26"/>
+      <c r="O83" s="24"/>
       <c r="P83" s="25"/>
       <c r="Q83" s="25"/>
       <c r="R83" s="25"/>
@@ -2201,24 +2215,24 @@
     <row r="90" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="91" spans="1:19" ht="30" customHeight="1">
       <c r="A91" s="1"/>
-      <c r="B91" s="27" t="s">
+      <c r="B91" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C91" s="21">
         <v>45655</v>
       </c>
       <c r="D91" s="22"/>
-      <c r="E91" s="26"/>
+      <c r="E91" s="24"/>
       <c r="F91" s="25"/>
       <c r="G91" s="25"/>
       <c r="H91" s="25"/>
       <c r="I91" s="25"/>
-      <c r="J91" s="26"/>
+      <c r="J91" s="24"/>
       <c r="K91" s="25"/>
       <c r="L91" s="25"/>
       <c r="M91" s="25"/>
       <c r="N91" s="25"/>
-      <c r="O91" s="26"/>
+      <c r="O91" s="24"/>
       <c r="P91" s="25"/>
       <c r="Q91" s="25"/>
       <c r="R91" s="25"/>
@@ -2287,18 +2301,30 @@
         <v>SATURDAY</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="12.75">
+    <row r="94" spans="1:19" ht="63.75">
       <c r="A94" s="11"/>
       <c r="B94" s="12"/>
       <c r="C94" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-      <c r="F94" s="19"/>
-      <c r="G94" s="19"/>
-      <c r="H94" s="19"/>
-      <c r="I94" s="19"/>
+      <c r="D94" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F94" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G94" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H94" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I94" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="95" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="96" spans="1:19" ht="15.75" customHeight="1"/>
@@ -3208,15 +3234,11 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E91:I91"/>
-    <mergeCell ref="J91:N91"/>
-    <mergeCell ref="O91:S91"/>
-    <mergeCell ref="E75:I75"/>
-    <mergeCell ref="J75:N75"/>
-    <mergeCell ref="O75:S75"/>
-    <mergeCell ref="E83:I83"/>
-    <mergeCell ref="J83:N83"/>
-    <mergeCell ref="O83:S83"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="E67:I67"/>
     <mergeCell ref="J67:N67"/>
     <mergeCell ref="O67:S67"/>
@@ -3228,13 +3250,17 @@
     <mergeCell ref="E51:I51"/>
     <mergeCell ref="J51:N51"/>
     <mergeCell ref="O51:S51"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E91:I91"/>
+    <mergeCell ref="J91:N91"/>
+    <mergeCell ref="O91:S91"/>
+    <mergeCell ref="E75:I75"/>
+    <mergeCell ref="J75:N75"/>
+    <mergeCell ref="O75:S75"/>
+    <mergeCell ref="E83:I83"/>
+    <mergeCell ref="J83:N83"/>
+    <mergeCell ref="O83:S83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update LichLamViec 26/1 - 7/2
</commit_message>
<xml_diff>
--- a/5_TaskList/Lịch làm việc.xlsx
+++ b/5_TaskList/Lịch làm việc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
   <si>
     <t xml:space="preserve">Tuần: 01
 </t>
@@ -301,7 +301,30 @@
 </t>
   </si>
   <si>
-    <t>Tiềm hiểu về cách cào dữ liệu từ trang web khác bằng cách đọc html.</t>
+    <t>Tiềm hiểu về cách cào dữ liệu từ trang web khác bằng cách đọc html. Tìm hiểu về CrystalReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuần: 16
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuần: 17
+</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Vue.js. Chỉnh lại form SendMessToAsset chọn địa chỉ BootstrapServer (FOX, LLQ)</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Vue.js.</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Vue.js. Về component</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Vue.js, Về hiệu ứng chuyển động</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm hiểu về Vue.js. Về component </t>
   </si>
 </sst>
 </file>
@@ -771,8 +794,8 @@
   </sheetPr>
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -2698,7 +2721,7 @@
         <v>SATURDAY</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="51">
+    <row r="119" spans="1:19" ht="63.75">
       <c r="A119" s="11"/>
       <c r="B119" s="12"/>
       <c r="C119" s="19" t="s">
@@ -2707,7 +2730,9 @@
       <c r="D119" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E119" s="19"/>
+      <c r="E119" s="19" t="s">
+        <v>2</v>
+      </c>
       <c r="F119" s="19" t="s">
         <v>2</v>
       </c>
@@ -2724,28 +2749,246 @@
     <row r="120" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="121" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="122" spans="1:19" ht="15.75" customHeight="1"/>
-    <row r="123" spans="1:19" ht="15.75" customHeight="1"/>
-    <row r="124" spans="1:19" ht="15.75" customHeight="1"/>
-    <row r="125" spans="1:19" ht="15.75" customHeight="1"/>
-    <row r="126" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="123" spans="1:19" ht="30" customHeight="1">
+      <c r="A123" s="1"/>
+      <c r="B123" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C123" s="21">
+        <v>45683</v>
+      </c>
+      <c r="D123" s="22"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="25"/>
+      <c r="H123" s="25"/>
+      <c r="I123" s="25"/>
+      <c r="J123" s="24"/>
+      <c r="K123" s="25"/>
+      <c r="L123" s="25"/>
+      <c r="M123" s="25"/>
+      <c r="N123" s="25"/>
+      <c r="O123" s="24"/>
+      <c r="P123" s="25"/>
+      <c r="Q123" s="25"/>
+      <c r="R123" s="25"/>
+      <c r="S123" s="25"/>
+    </row>
+    <row r="124" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="8">
+        <f>C123</f>
+        <v>45683</v>
+      </c>
+      <c r="D124" s="8">
+        <f>C123+1</f>
+        <v>45684</v>
+      </c>
+      <c r="E124" s="8">
+        <f>C123+2</f>
+        <v>45685</v>
+      </c>
+      <c r="F124" s="8">
+        <f>C123+3</f>
+        <v>45686</v>
+      </c>
+      <c r="G124" s="8">
+        <f>C123+4</f>
+        <v>45687</v>
+      </c>
+      <c r="H124" s="8">
+        <f>C123+5</f>
+        <v>45688</v>
+      </c>
+      <c r="I124" s="8">
+        <f>C123+6</f>
+        <v>45689</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A125" s="9"/>
+      <c r="C125" s="10" t="str">
+        <f t="shared" ref="C125:I125" si="16">UPPER(TEXT(C124, "DDDD"))</f>
+        <v>SUNDAY</v>
+      </c>
+      <c r="D125" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>MONDAY</v>
+      </c>
+      <c r="E125" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>TUESDAY</v>
+      </c>
+      <c r="F125" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>WEDNESDAY</v>
+      </c>
+      <c r="G125" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>THURSDAY</v>
+      </c>
+      <c r="H125" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>FRIDAY</v>
+      </c>
+      <c r="I125" s="10" t="str">
+        <f t="shared" si="16"/>
+        <v>SATURDAY</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" ht="12.75">
+      <c r="A126" s="11"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="I126" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="127" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="128" spans="1:19" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="129" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="130" spans="1:19" ht="30" customHeight="1">
+      <c r="A130" s="1"/>
+      <c r="B130" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C130" s="21">
+        <v>45690</v>
+      </c>
+      <c r="D130" s="22"/>
+      <c r="E130" s="24"/>
+      <c r="F130" s="25"/>
+      <c r="G130" s="25"/>
+      <c r="H130" s="25"/>
+      <c r="I130" s="25"/>
+      <c r="J130" s="24"/>
+      <c r="K130" s="25"/>
+      <c r="L130" s="25"/>
+      <c r="M130" s="25"/>
+      <c r="N130" s="25"/>
+      <c r="O130" s="24"/>
+      <c r="P130" s="25"/>
+      <c r="Q130" s="25"/>
+      <c r="R130" s="25"/>
+      <c r="S130" s="25"/>
+    </row>
+    <row r="131" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="8">
+        <f>C130</f>
+        <v>45690</v>
+      </c>
+      <c r="D131" s="8">
+        <f>C130+1</f>
+        <v>45691</v>
+      </c>
+      <c r="E131" s="8">
+        <f>C130+2</f>
+        <v>45692</v>
+      </c>
+      <c r="F131" s="8">
+        <f>C130+3</f>
+        <v>45693</v>
+      </c>
+      <c r="G131" s="8">
+        <f>C130+4</f>
+        <v>45694</v>
+      </c>
+      <c r="H131" s="8">
+        <f>C130+5</f>
+        <v>45695</v>
+      </c>
+      <c r="I131" s="8">
+        <f>C130+6</f>
+        <v>45696</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A132" s="9"/>
+      <c r="C132" s="10" t="str">
+        <f t="shared" ref="C132:I132" si="17">UPPER(TEXT(C131, "DDDD"))</f>
+        <v>SUNDAY</v>
+      </c>
+      <c r="D132" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>MONDAY</v>
+      </c>
+      <c r="E132" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>TUESDAY</v>
+      </c>
+      <c r="F132" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>WEDNESDAY</v>
+      </c>
+      <c r="G132" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>THURSDAY</v>
+      </c>
+      <c r="H132" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>FRIDAY</v>
+      </c>
+      <c r="I132" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v>SATURDAY</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" ht="63.75">
+      <c r="A133" s="11"/>
+      <c r="B133" s="12"/>
+      <c r="C133" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E133" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F133" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G133" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H133" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I133" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="135" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="136" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="137" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="138" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="139" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="140" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="141" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="142" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="143" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="144" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1"/>
     <row r="146" ht="15.75" customHeight="1"/>
     <row r="147" ht="15.75" customHeight="1"/>
@@ -3603,7 +3846,31 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="40">
+    <mergeCell ref="E123:I123"/>
+    <mergeCell ref="J123:N123"/>
+    <mergeCell ref="O123:S123"/>
+    <mergeCell ref="E130:I130"/>
+    <mergeCell ref="J130:N130"/>
+    <mergeCell ref="O130:S130"/>
+    <mergeCell ref="E99:I99"/>
+    <mergeCell ref="J99:N99"/>
+    <mergeCell ref="O99:S99"/>
+    <mergeCell ref="E108:I108"/>
+    <mergeCell ref="J108:N108"/>
+    <mergeCell ref="O108:S108"/>
+    <mergeCell ref="E51:I51"/>
+    <mergeCell ref="J51:N51"/>
+    <mergeCell ref="O51:S51"/>
+    <mergeCell ref="E91:I91"/>
+    <mergeCell ref="J91:N91"/>
+    <mergeCell ref="O91:S91"/>
+    <mergeCell ref="E75:I75"/>
+    <mergeCell ref="J75:N75"/>
+    <mergeCell ref="O75:S75"/>
+    <mergeCell ref="E83:I83"/>
+    <mergeCell ref="J83:N83"/>
+    <mergeCell ref="O83:S83"/>
     <mergeCell ref="E116:I116"/>
     <mergeCell ref="J116:N116"/>
     <mergeCell ref="O116:S116"/>
@@ -3620,24 +3887,6 @@
     <mergeCell ref="E59:I59"/>
     <mergeCell ref="J59:N59"/>
     <mergeCell ref="O59:S59"/>
-    <mergeCell ref="E51:I51"/>
-    <mergeCell ref="J51:N51"/>
-    <mergeCell ref="O51:S51"/>
-    <mergeCell ref="E91:I91"/>
-    <mergeCell ref="J91:N91"/>
-    <mergeCell ref="O91:S91"/>
-    <mergeCell ref="E75:I75"/>
-    <mergeCell ref="J75:N75"/>
-    <mergeCell ref="O75:S75"/>
-    <mergeCell ref="E83:I83"/>
-    <mergeCell ref="J83:N83"/>
-    <mergeCell ref="O83:S83"/>
-    <mergeCell ref="E99:I99"/>
-    <mergeCell ref="J99:N99"/>
-    <mergeCell ref="O99:S99"/>
-    <mergeCell ref="E108:I108"/>
-    <mergeCell ref="J108:N108"/>
-    <mergeCell ref="O108:S108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update LichLamViec 20/4 -3
</commit_message>
<xml_diff>
--- a/5_TaskList/Lịch làm việc.xlsx
+++ b/5_TaskList/Lịch làm việc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="151">
   <si>
     <t xml:space="preserve">Tuần: 01
 </t>
@@ -448,9 +448,6 @@
     <t>Tạo Cụm fitthuctap14 với địa chỉ Host tại máy mình (10.26.4.44:9092). Test gửi mess đến (thành công)</t>
   </si>
   <si>
-    <t>Dựng Kafka ui bằng Docker Compos. Tạo Cụm FPTS (10.26.7.58:9092,10.26.7.59:9092,10.26.7.60:9092)</t>
-  </si>
-  <si>
     <t>Đọc và tìm hiểu các sp trong mamo_test. thêm định dạng số nhập vào của form điều chỉnh hạn mực đặc biệt</t>
   </si>
   <si>
@@ -504,6 +501,35 @@
   </si>
   <si>
     <t>Xem lại code form điều chỉnh hạn mức xem có bỏ được binding redirects không (Không vì Npgsql 5.0.18.0 không hỗ trợ các thư viên đó ở phiên bản cao hơn, không cài bản Npgsql cao hơn vì đạng sử dụng .NET Framework 4.7)</t>
+  </si>
+  <si>
+    <t>Dựng Kafka ui bằng Docker Compose. Tạo Cụm FPTS (10.26.7.58:9092,10.26.7.59:9092,10.26.7.60:9092)</t>
+  </si>
+  <si>
+    <t>Thử tạo giao diện trang báo cáo tài sản                  Nghỉ chiều</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thử tạo giao diện trang báo cáo tài sản                  </t>
+  </si>
+  <si>
+    <t>Nghiên cứu API Query Parameters (pagination, Caching)                                 Nghỉ chiều.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuần: 26
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuần: 27
+</t>
+  </si>
+  <si>
+    <t>Nghiên cứu code gia hạn, trả nợ</t>
+  </si>
+  <si>
+    <t>Nghiên cứu code cầm cố, gia hạn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm hiểu nghiệp vụ của mua, bán CK trên web, cầm cố, gia hạn, trả nợ bản dev. </t>
   </si>
 </sst>
 </file>
@@ -976,8 +1002,8 @@
   </sheetPr>
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H207" sqref="H207"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N222" sqref="N222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1966,7 +1992,7 @@
         <v>SATURDAY</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="102">
+    <row r="54" spans="1:19" ht="89.25">
       <c r="A54" s="11"/>
       <c r="B54" s="12"/>
       <c r="C54" s="19" t="s">
@@ -2200,7 +2226,7 @@
         <v>SATURDAY</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="89.25">
+    <row r="70" spans="1:19" ht="76.5">
       <c r="A70" s="11"/>
       <c r="B70" s="12"/>
       <c r="C70" s="19" t="s">
@@ -2668,7 +2694,7 @@
         <v>SATURDAY</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="89.25">
+    <row r="102" spans="1:19" ht="76.5">
       <c r="A102" s="11"/>
       <c r="B102" s="12"/>
       <c r="C102" s="19" t="s">
@@ -3959,19 +3985,19 @@
         <v>2</v>
       </c>
       <c r="D182" s="24" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="E182" s="24" t="s">
         <v>123</v>
       </c>
       <c r="F182" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G182" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="H182" s="24" t="s">
         <v>126</v>
-      </c>
-      <c r="G182" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H182" s="24" t="s">
-        <v>127</v>
       </c>
       <c r="I182" s="24" t="s">
         <v>2</v>
@@ -3988,7 +4014,7 @@
     <row r="186" spans="1:19" ht="30" customHeight="1">
       <c r="A186" s="1"/>
       <c r="B186" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C186" s="21">
         <v>45746</v>
@@ -4080,19 +4106,19 @@
         <v>2</v>
       </c>
       <c r="D189" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E189" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="F189" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G189" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="E189" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="F189" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="G189" s="24" t="s">
+      <c r="H189" s="24" t="s">
         <v>132</v>
-      </c>
-      <c r="H189" s="24" t="s">
-        <v>133</v>
       </c>
       <c r="I189" s="24" t="s">
         <v>2</v>
@@ -4110,7 +4136,7 @@
     <row r="194" spans="1:19" ht="30" customHeight="1">
       <c r="A194" s="1"/>
       <c r="B194" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C194" s="21">
         <v>45753</v>
@@ -4202,19 +4228,19 @@
         <v>2</v>
       </c>
       <c r="D197" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E197" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F197" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="E197" s="24" t="s">
+      <c r="G197" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="F197" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="G197" s="24" t="s">
+      <c r="H197" s="24" t="s">
         <v>137</v>
-      </c>
-      <c r="H197" s="24" t="s">
-        <v>138</v>
       </c>
       <c r="I197" s="24" t="s">
         <v>2</v>
@@ -4232,7 +4258,7 @@
     <row r="202" spans="1:19" ht="30" customHeight="1">
       <c r="A202" s="1"/>
       <c r="B202" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C202" s="21">
         <v>45760</v>
@@ -4324,19 +4350,19 @@
         <v>2</v>
       </c>
       <c r="D205" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E205" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F205" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="G205" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E205" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F205" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="G205" s="24" t="s">
+      <c r="H205" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="H205" s="24" t="s">
-        <v>141</v>
       </c>
       <c r="I205" s="24" t="s">
         <v>2</v>
@@ -4350,22 +4376,248 @@
     <row r="206" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="207" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="208" spans="1:19" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="209" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="210" spans="1:19" ht="30" customHeight="1">
+      <c r="A210" s="1"/>
+      <c r="B210" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C210" s="21">
+        <v>45767</v>
+      </c>
+      <c r="D210" s="22"/>
+      <c r="E210" s="25"/>
+      <c r="F210" s="26"/>
+      <c r="G210" s="26"/>
+      <c r="H210" s="26"/>
+      <c r="I210" s="26"/>
+      <c r="J210" s="25"/>
+      <c r="K210" s="26"/>
+      <c r="L210" s="26"/>
+      <c r="M210" s="26"/>
+      <c r="N210" s="26"/>
+      <c r="O210" s="25"/>
+      <c r="P210" s="26"/>
+      <c r="Q210" s="26"/>
+      <c r="R210" s="26"/>
+      <c r="S210" s="26"/>
+    </row>
+    <row r="211" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A211" s="7"/>
+      <c r="B211" s="7"/>
+      <c r="C211" s="8">
+        <f>C210</f>
+        <v>45767</v>
+      </c>
+      <c r="D211" s="8">
+        <f>C210+1</f>
+        <v>45768</v>
+      </c>
+      <c r="E211" s="8">
+        <f>C210+2</f>
+        <v>45769</v>
+      </c>
+      <c r="F211" s="8">
+        <f>C210+3</f>
+        <v>45770</v>
+      </c>
+      <c r="G211" s="8">
+        <f>C210+4</f>
+        <v>45771</v>
+      </c>
+      <c r="H211" s="8">
+        <f>C210+5</f>
+        <v>45772</v>
+      </c>
+      <c r="I211" s="8">
+        <f>C210+6</f>
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A212" s="9"/>
+      <c r="C212" s="10" t="str">
+        <f t="shared" ref="C212:I212" si="28">UPPER(TEXT(C211, "DDDD"))</f>
+        <v>SUNDAY</v>
+      </c>
+      <c r="D212" s="10" t="str">
+        <f t="shared" si="28"/>
+        <v>MONDAY</v>
+      </c>
+      <c r="E212" s="10" t="str">
+        <f t="shared" si="28"/>
+        <v>TUESDAY</v>
+      </c>
+      <c r="F212" s="10" t="str">
+        <f t="shared" si="28"/>
+        <v>WEDNESDAY</v>
+      </c>
+      <c r="G212" s="10" t="str">
+        <f t="shared" si="28"/>
+        <v>THURSDAY</v>
+      </c>
+      <c r="H212" s="10" t="str">
+        <f t="shared" si="28"/>
+        <v>FRIDAY</v>
+      </c>
+      <c r="I212" s="10" t="str">
+        <f t="shared" si="28"/>
+        <v>SATURDAY</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" ht="51">
+      <c r="A213" s="11"/>
+      <c r="B213" s="12"/>
+      <c r="C213" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D213" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E213" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F213" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G213" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="H213" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="I213" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J213" s="24"/>
+      <c r="K213" s="12"/>
+      <c r="L213" s="12"/>
+      <c r="M213" s="12"/>
+      <c r="N213" s="12"/>
+    </row>
+    <row r="214" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="215" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="216" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="217" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="218" spans="1:19" ht="30" customHeight="1">
+      <c r="A218" s="1"/>
+      <c r="B218" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C218" s="21">
+        <v>45774</v>
+      </c>
+      <c r="D218" s="22"/>
+      <c r="E218" s="25"/>
+      <c r="F218" s="26"/>
+      <c r="G218" s="26"/>
+      <c r="H218" s="26"/>
+      <c r="I218" s="26"/>
+      <c r="J218" s="25"/>
+      <c r="K218" s="26"/>
+      <c r="L218" s="26"/>
+      <c r="M218" s="26"/>
+      <c r="N218" s="26"/>
+      <c r="O218" s="25"/>
+      <c r="P218" s="26"/>
+      <c r="Q218" s="26"/>
+      <c r="R218" s="26"/>
+      <c r="S218" s="26"/>
+    </row>
+    <row r="219" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A219" s="7"/>
+      <c r="B219" s="7"/>
+      <c r="C219" s="8">
+        <f>C218</f>
+        <v>45774</v>
+      </c>
+      <c r="D219" s="8">
+        <f>C218+1</f>
+        <v>45775</v>
+      </c>
+      <c r="E219" s="8">
+        <f>C218+2</f>
+        <v>45776</v>
+      </c>
+      <c r="F219" s="8">
+        <f>C218+3</f>
+        <v>45777</v>
+      </c>
+      <c r="G219" s="8">
+        <f>C218+4</f>
+        <v>45778</v>
+      </c>
+      <c r="H219" s="8">
+        <f>C218+5</f>
+        <v>45779</v>
+      </c>
+      <c r="I219" s="8">
+        <f>C218+6</f>
+        <v>45780</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A220" s="9"/>
+      <c r="C220" s="10" t="str">
+        <f t="shared" ref="C220:I220" si="29">UPPER(TEXT(C219, "DDDD"))</f>
+        <v>SUNDAY</v>
+      </c>
+      <c r="D220" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>MONDAY</v>
+      </c>
+      <c r="E220" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>TUESDAY</v>
+      </c>
+      <c r="F220" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>WEDNESDAY</v>
+      </c>
+      <c r="G220" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>THURSDAY</v>
+      </c>
+      <c r="H220" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>FRIDAY</v>
+      </c>
+      <c r="I220" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>SATURDAY</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19" ht="51">
+      <c r="A221" s="11"/>
+      <c r="B221" s="12"/>
+      <c r="C221" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D221" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E221" s="24"/>
+      <c r="F221" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G221" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="H221" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I221" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="J221" s="24"/>
+      <c r="K221" s="12"/>
+      <c r="L221" s="12"/>
+      <c r="M221" s="12"/>
+      <c r="N221" s="12"/>
+    </row>
+    <row r="222" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="223" spans="1:19" ht="15.75" customHeight="1"/>
+    <row r="224" spans="1:19" ht="15.75" customHeight="1"/>
     <row r="225" ht="15.75" customHeight="1"/>
     <row r="226" ht="15.75" customHeight="1"/>
     <row r="227" ht="15.75" customHeight="1"/>
@@ -5143,7 +5395,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="76">
     <mergeCell ref="E137:I137"/>
     <mergeCell ref="J137:N137"/>
     <mergeCell ref="O137:S137"/>
@@ -5214,6 +5466,12 @@
     <mergeCell ref="E202:I202"/>
     <mergeCell ref="J202:N202"/>
     <mergeCell ref="O202:S202"/>
+    <mergeCell ref="E210:I210"/>
+    <mergeCell ref="J210:N210"/>
+    <mergeCell ref="O210:S210"/>
+    <mergeCell ref="E218:I218"/>
+    <mergeCell ref="J218:N218"/>
+    <mergeCell ref="O218:S218"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>